<commit_message>
order by kode cpmk
</commit_message>
<xml_diff>
--- a/backend/modules/import/templates/template-nilai.xlsx
+++ b/backend/modules/import/templates/template-nilai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\iabee\backend\modules\import\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAE0FE8-9039-4081-9F03-7DD0621BE755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9E2EC3-9BBE-420A-83D2-5D47DBA748D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{8D77FA8A-F331-40F0-9C72-F1E9CF6A7C60}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B72AD4E-E665-4320-9E1D-59F2EE0EC394}">
   <dimension ref="A2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>